<commit_message>
WIP Speeding up annual energy and cost calculations
</commit_message>
<xml_diff>
--- a/Data/Cost_estimation.xlsx
+++ b/Data/Cost_estimation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s124129\Documents\GitHub\Brabant-buurt-serious-game\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BAE5DC0-8DE6-4736-B4AF-630E8D29A8A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAEADF30-DFB4-4DB3-8067-CAD7A205B740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{692682D6-B432-47D6-B814-AA5FB880D973}"/>
+    <workbookView xWindow="-23148" yWindow="552" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{692682D6-B432-47D6-B814-AA5FB880D973}"/>
   </bookViews>
   <sheets>
     <sheet name="Inhouse heat systems" sheetId="1" r:id="rId1"/>
@@ -430,7 +430,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -512,7 +512,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -855,16 +855,16 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -890,7 +890,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -916,7 +916,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -942,7 +942,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -968,7 +968,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -994,7 +994,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1020,7 +1020,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>42</v>
       </c>
@@ -1043,7 +1043,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>43</v>
       </c>
@@ -1066,7 +1066,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -1100,22 +1100,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E437254-8431-436A-A556-48E8AFAFCC33}">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -1156,7 +1156,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1194,11 +1194,11 @@
         <v>50</v>
       </c>
       <c r="M2" s="7">
-        <f>L2/3.6/1000</f>
-        <v>1.388888888888889E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+        <f>L2*3.6/1000</f>
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1236,11 +1236,11 @@
         <v>50</v>
       </c>
       <c r="M3" s="7">
-        <f t="shared" ref="M3:M5" si="0">L3/3.6/1000</f>
-        <v>1.388888888888889E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+        <f t="shared" ref="M3:M5" si="0">L3*3.6/1000</f>
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1279,10 +1279,10 @@
       </c>
       <c r="M4" s="7">
         <f t="shared" si="0"/>
-        <v>1.388888888888889E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -1321,7 +1321,7 @@
       </c>
       <c r="M5" s="7">
         <f t="shared" si="0"/>
-        <v>1.388888888888889E-2</v>
+        <v>0.18</v>
       </c>
     </row>
   </sheetData>
@@ -1338,14 +1338,14 @@
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
@@ -1359,7 +1359,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1373,7 +1373,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -1387,7 +1387,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -1401,7 +1401,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -1415,7 +1415,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -1442,15 +1442,15 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>33</v>
       </c>
@@ -1464,7 +1464,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -1478,7 +1478,7 @@
         <v>0.108</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>0.113</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -1506,7 +1506,7 @@
         <v>0.126</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -1520,7 +1520,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -1547,18 +1547,18 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>69</v>
       </c>
@@ -1590,7 +1590,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2018</v>
       </c>
@@ -1624,7 +1624,7 @@
         <v>0.21779999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2019</v>
       </c>
@@ -1658,7 +1658,7 @@
         <v>0.22989999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -1692,7 +1692,7 @@
         <v>0.22989999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2022</v>
       </c>
@@ -1726,7 +1726,7 @@
         <v>0.77063000000000015</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2030</v>
       </c>
@@ -1773,14 +1773,14 @@
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>49</v>
       </c>
@@ -1800,7 +1800,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -1820,7 +1820,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -1840,7 +1840,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>55</v>
       </c>
@@ -1860,7 +1860,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -1880,7 +1880,7 @@
         <v>6500</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -1900,7 +1900,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>56</v>
       </c>
@@ -1920,7 +1920,7 @@
         <v>16000</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>57</v>
       </c>
@@ -1940,7 +1940,7 @@
         <v>4400</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>57</v>
       </c>
@@ -1960,7 +1960,7 @@
         <v>9500</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>57</v>
       </c>
@@ -1980,7 +1980,7 @@
         <v>9600</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -2000,7 +2000,7 @@
         <v>7800</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>58</v>
       </c>
@@ -2020,7 +2020,7 @@
         <v>24000</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>58</v>
       </c>
@@ -2040,7 +2040,7 @@
         <v>19200</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>59</v>
       </c>
@@ -2060,7 +2060,7 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>59</v>
       </c>
@@ -2080,7 +2080,7 @@
         <v>34000</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>59</v>
       </c>
@@ -2114,19 +2114,19 @@
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.21875" customWidth="1"/>
-    <col min="2" max="2" width="28.109375" customWidth="1"/>
-    <col min="3" max="3" width="29.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="13.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" customWidth="1"/>
+    <col min="3" max="3" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>80</v>
       </c>
@@ -2158,7 +2158,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>81</v>
       </c>
@@ -2192,7 +2192,7 @@
         <v>0.68788499999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>81</v>
       </c>
@@ -2226,7 +2226,7 @@
         <v>0.76520399999999988</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>81</v>
       </c>
@@ -2260,7 +2260,7 @@
         <v>0.80767500000000014</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>81</v>
       </c>
@@ -2294,7 +2294,7 @@
         <v>2.9602649999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>81</v>
       </c>
@@ -2328,7 +2328,7 @@
         <v>1.0164</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>82</v>
       </c>
@@ -2363,7 +2363,7 @@
         <v>1.7866860000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>82</v>
       </c>
@@ -2398,7 +2398,7 @@
         <v>1.8229860000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>82</v>
       </c>
@@ -2433,7 +2433,7 @@
         <v>1.8713860000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>82</v>
       </c>
@@ -2468,7 +2468,7 @@
         <v>1.8713860000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>82</v>
       </c>
@@ -2518,12 +2518,12 @@
       <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>76</v>
       </c>
@@ -2537,7 +2537,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>57</v>
       </c>
@@ -2551,7 +2551,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -2565,7 +2565,7 @@
         <v>0.69</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>59</v>
       </c>
@@ -2579,7 +2579,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -2593,7 +2593,7 @@
         <v>0.69</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>55</v>
       </c>

</xml_diff>

<commit_message>
WIP heating  system simplification and energy calculations
</commit_message>
<xml_diff>
--- a/Data/Cost_estimation.xlsx
+++ b/Data/Cost_estimation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s124129\Documents\GitHub\Brabant-buurt-serious-game\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A34DB84-0B94-45EA-9D23-89579486080A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52FFA77C-A4B0-4C85-AE4C-9C5F1CB36EF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{692682D6-B432-47D6-B814-AA5FB880D973}"/>
+    <workbookView xWindow="3048" yWindow="732" windowWidth="17280" windowHeight="9060" xr2:uid="{692682D6-B432-47D6-B814-AA5FB880D973}"/>
   </bookViews>
   <sheets>
     <sheet name="Inhouse heat systems" sheetId="1" r:id="rId1"/>
@@ -102,7 +102,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="106">
   <si>
     <t>Unit</t>
   </si>
@@ -428,6 +428,21 @@
   </si>
   <si>
     <t>See energievraag en isolatie woningen</t>
+  </si>
+  <si>
+    <t>LT-Warmtenet</t>
+  </si>
+  <si>
+    <t>MT-Warmtenet</t>
+  </si>
+  <si>
+    <t>Verlies</t>
+  </si>
+  <si>
+    <t>Electric boiler</t>
+  </si>
+  <si>
+    <t>EUR per aansluiting</t>
   </si>
 </sst>
 </file>
@@ -855,22 +870,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C01DEAE-B245-4BB5-9FCD-4FA4EE9440AC}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -896,7 +911,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -922,7 +937,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -948,7 +963,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -974,7 +989,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1000,7 +1015,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1026,9 +1041,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>104</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1040,18 +1058,19 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>8</v>
+        <f>(1774.85+1112)/2</f>
+        <v>1443.425</v>
       </c>
       <c r="G7" t="s">
-        <v>46</v>
+        <v>105</v>
       </c>
       <c r="H7">
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -1063,7 +1082,7 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G8" t="s">
         <v>46</v>
@@ -1072,9 +1091,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1086,21 +1105,18 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>71</v>
+        <v>15</v>
       </c>
       <c r="G9" t="s">
         <v>46</v>
       </c>
       <c r="H9">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>99</v>
-      </c>
-      <c r="B10" t="s">
-        <v>100</v>
+        <v>44</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -1112,12 +1128,38 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>71</v>
       </c>
       <c r="G10" t="s">
         <v>46</v>
       </c>
       <c r="H10">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11">
         <v>30</v>
       </c>
     </row>
@@ -1130,24 +1172,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E437254-8431-436A-A556-48E8AFAFCC33}">
-  <dimension ref="A1:M5"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="36.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="36.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -1187,8 +1229,11 @@
       <c r="M1" s="2" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -1229,8 +1274,11 @@
         <f>L2*3.6/1000</f>
         <v>0.18</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N2" s="6">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -1271,8 +1319,11 @@
         <f t="shared" ref="M3:M5" si="0">L3*3.6/1000</f>
         <v>0.18</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N3" s="6">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1313,10 +1364,13 @@
         <f t="shared" si="0"/>
         <v>0.18</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N4" s="6">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>101</v>
       </c>
       <c r="B5">
         <v>270</v>
@@ -1354,6 +1408,54 @@
       <c r="M5" s="7">
         <f t="shared" si="0"/>
         <v>0.18</v>
+      </c>
+      <c r="N5" s="6">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B6">
+        <v>271</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="6">
+        <v>271</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="I6" s="6">
+        <v>0</v>
+      </c>
+      <c r="J6" s="6">
+        <v>0</v>
+      </c>
+      <c r="K6" s="6">
+        <v>30</v>
+      </c>
+      <c r="L6" s="6">
+        <v>50</v>
+      </c>
+      <c r="M6" s="7">
+        <f t="shared" ref="M6" si="1">L6*3.6/1000</f>
+        <v>0.18</v>
+      </c>
+      <c r="N6" s="6">
+        <v>0.3</v>
       </c>
     </row>
   </sheetData>
@@ -1370,14 +1472,14 @@
       <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>21</v>
       </c>
@@ -1391,7 +1493,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -1405,7 +1507,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -1419,7 +1521,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>28</v>
       </c>
@@ -1433,7 +1535,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -1447,7 +1549,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -1471,18 +1573,18 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>33</v>
       </c>
@@ -1496,7 +1598,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -1510,7 +1612,7 @@
         <v>0.108</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -1524,7 +1626,7 @@
         <v>0.113</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -1538,7 +1640,7 @@
         <v>0.126</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -1552,7 +1654,7 @@
         <v>8.5999999999999993E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -1576,21 +1678,21 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>69</v>
       </c>
@@ -1622,7 +1724,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2018</v>
       </c>
@@ -1656,7 +1758,7 @@
         <v>0.21779999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2019</v>
       </c>
@@ -1690,7 +1792,7 @@
         <v>0.22989999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2020</v>
       </c>
@@ -1724,7 +1826,7 @@
         <v>0.22989999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>2022</v>
       </c>
@@ -1758,7 +1860,7 @@
         <v>0.77063000000000015</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2030</v>
       </c>
@@ -1805,14 +1907,14 @@
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>49</v>
       </c>
@@ -1832,7 +1934,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -1852,7 +1954,7 @@
         <v>5400</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -1872,7 +1974,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>55</v>
       </c>
@@ -1892,7 +1994,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -1912,7 +2014,7 @@
         <v>6500</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>56</v>
       </c>
@@ -1932,7 +2034,7 @@
         <v>20000</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>56</v>
       </c>
@@ -1952,7 +2054,7 @@
         <v>16000</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>57</v>
       </c>
@@ -1972,7 +2074,7 @@
         <v>4400</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>57</v>
       </c>
@@ -1992,7 +2094,7 @@
         <v>9500</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>57</v>
       </c>
@@ -2012,7 +2114,7 @@
         <v>9600</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>58</v>
       </c>
@@ -2032,7 +2134,7 @@
         <v>7800</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>58</v>
       </c>
@@ -2052,7 +2154,7 @@
         <v>24000</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>58</v>
       </c>
@@ -2072,7 +2174,7 @@
         <v>19200</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>59</v>
       </c>
@@ -2092,7 +2194,7 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>59</v>
       </c>
@@ -2112,7 +2214,7 @@
         <v>34000</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>59</v>
       </c>
@@ -2146,19 +2248,19 @@
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" customWidth="1"/>
-    <col min="2" max="2" width="28.140625" customWidth="1"/>
-    <col min="3" max="3" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="38.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="28.109375" customWidth="1"/>
+    <col min="3" max="3" width="29.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>80</v>
       </c>
@@ -2190,7 +2292,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>81</v>
       </c>
@@ -2224,7 +2326,7 @@
         <v>0.68788499999999997</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>81</v>
       </c>
@@ -2258,7 +2360,7 @@
         <v>0.76520399999999988</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>81</v>
       </c>
@@ -2292,7 +2394,7 @@
         <v>0.80767500000000014</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>81</v>
       </c>
@@ -2326,7 +2428,7 @@
         <v>2.9602649999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>81</v>
       </c>
@@ -2360,7 +2462,7 @@
         <v>1.0164</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>82</v>
       </c>
@@ -2395,7 +2497,7 @@
         <v>1.7866860000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>82</v>
       </c>
@@ -2430,7 +2532,7 @@
         <v>1.8229860000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>82</v>
       </c>
@@ -2465,7 +2567,7 @@
         <v>1.8713860000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>82</v>
       </c>
@@ -2500,7 +2602,7 @@
         <v>1.8713860000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>82</v>
       </c>
@@ -2550,12 +2652,12 @@
       <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>76</v>
       </c>
@@ -2569,7 +2671,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>57</v>
       </c>
@@ -2583,7 +2685,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -2597,7 +2699,7 @@
         <v>0.69</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>59</v>
       </c>
@@ -2611,7 +2713,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>58</v>
       </c>
@@ -2625,7 +2727,7 @@
         <v>0.69</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>55</v>
       </c>

</xml_diff>